<commit_message>
test chat with file
</commit_message>
<xml_diff>
--- a/backend/services/DataStructuring/DataStructuring/TargetData/图片.xlsx
+++ b/backend/services/DataStructuring/DataStructuring/TargetData/图片.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>单次</t>
         </is>
       </c>
     </row>
@@ -532,7 +532,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>34:49</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,16 @@
           <t>设备信息</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>设备信息指标：
+- 交易卡号：6222****4054
+- 交易账户：4301****1741
+- 对方账户：0019****0002
+- 交易国家或地区简称：CHN
+- 记账币种：人民币</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -558,7 +567,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>01-09 17:34:49</t>
         </is>
       </c>
     </row>
@@ -571,7 +580,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>它显示了交易发生的确切日期和时间</t>
         </is>
       </c>
     </row>
@@ -588,7 +597,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>794.97</t>
         </is>
       </c>
     </row>
@@ -601,7 +610,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>794.97</t>
         </is>
       </c>
     </row>
@@ -612,7 +621,20 @@
           <t>初始账户开户信息</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>开户时间：2025-01-09 17:34:49
+开户地点：网上银行
+交易卡号：6222****4054
+交易账户：4301****1741
+交易户名：朱晗
+记账金额：794.97
+记账币种：人民币
+对方账户：0019****0002
+对方户名：银联转账(云闪付)
+对方账户行别：上海银联电子支付服务有限公司</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -662,7 +684,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>网上银行用户</t>
         </is>
       </c>
     </row>
@@ -675,7 +697,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>收支详细信息</t>
         </is>
       </c>
     </row>
@@ -688,7 +710,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>6222****4054</t>
         </is>
       </c>
     </row>
@@ -705,7 +727,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>794.97</t>
         </is>
       </c>
     </row>
@@ -718,7 +740,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>794.97</t>
         </is>
       </c>
     </row>
@@ -729,7 +751,24 @@
           <t>目标账户开户信息</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>目标账户开户信息指标：
+- 开户时间：2025年1月9日17:34:49
+- 开户地点：网上银行
+- 交易卡号：6222****4054
+- 交易账户：4301****1741
+- 朱晗（交易者姓名）
+- 交易时间：2025年1月9日17:34:49
+- 业务摘要：无卡支付
+- 对方账户行别：上海银联电子支付服务有限公司
+- 对方账户：0019****0002
+- 银行代码：CHN
+- 交易金额：794.97
+- 记账币种：人民币
+- 记账金额：794.97</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -740,7 +779,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>未提供</t>
         </is>
       </c>
     </row>
@@ -753,7 +792,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>0019****0002</t>
         </is>
       </c>
     </row>
@@ -766,7 +805,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>开户日期</t>
         </is>
       </c>
     </row>
@@ -779,7 +818,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>朱晗的职业是网上银行交易</t>
         </is>
       </c>
     </row>
@@ -792,7 +831,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>不适用（因为没有提供与目标账户相关的受教育程度信息）</t>
         </is>
       </c>
     </row>
@@ -805,7 +844,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>对方面账户所有者注册的联系电话或电子邮件地址等</t>
         </is>
       </c>
     </row>
@@ -822,7 +861,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>否</t>
         </is>
       </c>
     </row>
@@ -835,7 +874,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>否</t>
         </is>
       </c>
     </row>

</xml_diff>